<commit_message>
Working image collection, no handler direct download
</commit_message>
<xml_diff>
--- a/Образец таблицы Партсбукинг.xlsx
+++ b/Образец таблицы Партсбукинг.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Артикул</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>R165605</t>
+  </si>
+  <si>
+    <t>John Deere</t>
   </si>
   <si>
     <t>Зубчатый венец</t>
@@ -591,10 +594,10 @@
         <v>14</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" s="8">
         <v>542659</v>
@@ -609,10 +612,10 @@
         <v>1269</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J3" s="8">
         <v>550932</v>
@@ -626,7 +629,7 @@
         <v>564208</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="9"/>
@@ -640,7 +643,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Changed Scraping algo, added Bandwidth log
</commit_message>
<xml_diff>
--- a/Образец таблицы Партсбукинг.xlsx
+++ b/Образец таблицы Партсбукинг.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Артикул</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>RE257192</t>
+  </si>
+  <si>
+    <t>R505452</t>
   </si>
 </sst>
 </file>
@@ -98,7 +101,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -158,11 +161,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -178,20 +184,20 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -506,209 +512,213 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="10" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="10" width="11.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="10" width="16.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="11" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="12" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="12" width="16.433571428571426" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="11" width="16.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="12" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="12" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="12" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="12" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="12" width="26.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="12" width="26.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="13" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="13" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="13" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="13" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="13" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="13" width="26.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="13" width="26.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="7" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="10">
         <v>192588</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="10">
         <v>3</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="10">
         <v>56260</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="10">
         <v>1463</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="10">
         <v>191137</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="10">
         <v>1434</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2" s="10">
         <v>194697</v>
       </c>
-      <c r="K2" s="8">
+      <c r="K2" s="10">
         <v>1520</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="7" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="10">
         <v>542659</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="10">
         <v>1</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="10">
         <v>542659</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="10">
         <v>1269</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="10">
         <v>550932</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="10">
         <v>1234</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="9">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="8">
         <v>564208</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="7" t="s">
+      <c r="C4" s="9"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>